<commit_message>
updates notes for NAs
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4C2FD9-E62B-0544-8B0E-980286DD2DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7D50EB-20B1-A849-AAF2-6F7589E06660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7540" yWindow="-19060" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30240" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>dateTime</t>
   </si>
   <si>
-    <t>YYYY-MM-DD hh:mm:ss</t>
-  </si>
-  <si>
     <t>Work that was done during visit to trap. Levels = c("Continue trapping", "Start trap &amp; begin trapping", "End trapping", "Unplanned restart", "Not applicable (n/a)", "Service/adjust/clean trap")</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>Trap position identifier</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -615,10 +615,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -767,10 +767,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
@@ -843,10 +843,10 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>25</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>26</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>27</v>
@@ -1122,10 +1122,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -1206,7 +1206,7 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>39</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>40</v>
@@ -1336,7 +1336,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="2"/>
       <c r="J20" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="3"/>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>42</v>
@@ -1376,7 +1376,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="2"/>
       <c r="J21" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="3"/>
@@ -1397,10 +1397,10 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>13</v>
@@ -1435,10 +1435,10 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
@@ -1473,10 +1473,10 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
@@ -28537,13 +28537,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>

</xml_diff>

<commit_message>
deletes wrong metadata files, removes old code from clean_data.R, and updates feather_catch_metadata.xlsx
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7D50EB-20B1-A849-AAF2-6F7589E06660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17398A08-9CDD-4541-B294-B712143ABBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -100,9 +100,6 @@
     <t>Foreign Key to the CAMP Release table</t>
   </si>
   <si>
-    <t>Run as assigned at the time of the capture.</t>
-  </si>
-  <si>
     <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis.</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>dateTime</t>
   </si>
   <si>
-    <t>Work that was done during visit to trap. Levels = c("Continue trapping", "Start trap &amp; begin trapping", "End trapping", "Unplanned restart", "Not applicable (n/a)", "Service/adjust/clean trap")</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -172,80 +166,59 @@
     <t>attribute_name</t>
   </si>
   <si>
-    <t>projectDescriptionID</t>
-  </si>
-  <si>
-    <t>taxonID</t>
-  </si>
-  <si>
-    <t>atCaptureRunID</t>
-  </si>
-  <si>
-    <t>atCaptureRunMethodID</t>
-  </si>
-  <si>
-    <t>finalRunID</t>
-  </si>
-  <si>
-    <t>finalRunMethodID</t>
-  </si>
-  <si>
-    <t>fishOriginID</t>
-  </si>
-  <si>
-    <t>lifeStageID</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>randomID</t>
-  </si>
-  <si>
-    <t>actualCountID</t>
-  </si>
-  <si>
-    <t>mortID</t>
-  </si>
-  <si>
-    <t>visitTime2</t>
-  </si>
-  <si>
-    <t>visitTypeID</t>
-  </si>
-  <si>
-    <t>siteID</t>
-  </si>
-  <si>
-    <t>trapPositionID</t>
-  </si>
-  <si>
     <t>Foreign key to the CAMP ProjectDescription table. All data associated with this package will have a ProjectDescriptionID = 2</t>
   </si>
   <si>
-    <t>Weight of the fish measured in grams</t>
+    <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>Taxon assigned</t>
+    <t>ProjectDescriptionID</t>
   </si>
   <si>
-    <t>Run method</t>
+    <t>siteName</t>
   </si>
   <si>
-    <t>Sampling site identifier</t>
+    <t>subSiteName</t>
   </si>
   <si>
-    <t>Trap position identifier</t>
+    <t>visitType</t>
   </si>
   <si>
-    <t>YYYY-MM-DD</t>
+    <t>commonName</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>fishOrigin</t>
+  </si>
+  <si>
+    <t>lifestage</t>
+  </si>
+  <si>
+    <t>mort</t>
+  </si>
+  <si>
+    <t>ActualCount</t>
+  </si>
+  <si>
+    <t>Name of the sampling site. Levels = c("Eye Riffle", "Live Oak", "Herringer Riffle")</t>
+  </si>
+  <si>
+    <t>Name of the trap or trap location. Levels = c("Eye riffle_north", "Live Oak", "Herringer_west", "Herringer_east", "Eye riffle_Side Channel")</t>
+  </si>
+  <si>
+    <t>Work that was done during visit to trap. Levels = c("Continue trapping", "Start trap &amp; begin trapping", "End trapping", "Unplanned restart")</t>
+  </si>
+  <si>
+    <t>Common name of species</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -263,6 +236,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -297,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,6 +304,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,11 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -618,7 +609,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -653,10 +644,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>18</v>
@@ -691,25 +682,27 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="5"/>
+      <c r="J4" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="K4" s="6"/>
       <c r="L4" s="7"/>
       <c r="M4" s="3"/>
@@ -729,19 +722,19 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -767,10 +760,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>66</v>
+      <c r="B6" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -785,9 +778,9 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="7"/>
       <c r="M6" s="3"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -805,10 +798,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
+      <c r="B7" s="11" t="s">
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -823,9 +816,9 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="3"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="7"/>
       <c r="M7" s="3"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -843,27 +836,27 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="3"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="7"/>
       <c r="M8" s="3"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -884,7 +877,7 @@
         <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -899,9 +892,9 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="3"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="7"/>
       <c r="M9" s="3"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -917,26 +910,29 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>53</v>
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="3"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
       <c r="M10" s="3"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -954,10 +950,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -972,9 +968,9 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="3"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
       <c r="M11" s="3"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -992,33 +988,27 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="7"/>
       <c r="M12" s="3"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1036,33 +1026,27 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="7"/>
       <c r="M13" s="3"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1080,31 +1064,27 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="H14" s="3"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="7"/>
       <c r="M14" s="3"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1122,31 +1102,33 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="7"/>
       <c r="M15" s="3"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1164,31 +1146,31 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="7"/>
       <c r="M16" s="3"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1206,45 +1188,52 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>57</v>
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
+      <c r="F17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="2"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1255,44 +1244,34 @@
       <c r="E18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="2"/>
       <c r="J18" s="5"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="1"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1316,28 +1295,16 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="J20" s="3"/>
       <c r="K20" s="2"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1356,28 +1323,16 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="1"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="2"/>
-      <c r="J21" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="J21" s="3"/>
       <c r="K21" s="2"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -1396,21 +1351,11 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A22" s="4"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1433,22 +1378,11 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>15</v>
-      </c>
+    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="1"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1472,21 +1406,11 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1538,6 +1462,7 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
@@ -1593,6 +1518,7 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
@@ -1649,31 +1575,30 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
-      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+      <c r="X30" s="4"/>
+      <c r="Y30" s="4"/>
+      <c r="Z30" s="4"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
@@ -1681,27 +1606,27 @@
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="4"/>
+      <c r="X31" s="4"/>
+      <c r="Y31" s="4"/>
+      <c r="Z31" s="4"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
@@ -1732,16 +1657,6 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="3"/>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1900,7 +1815,6 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1956,7 +1870,6 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -2572,7 +2485,7 @@
       <c r="Z62" s="1"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
+      <c r="A63" s="4"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="2"/>
@@ -2600,7 +2513,7 @@
       <c r="Z63" s="1"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
+      <c r="A64" s="4"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="2"/>
@@ -2628,7 +2541,7 @@
       <c r="Z64" s="1"/>
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1"/>
+      <c r="A65" s="4"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="2"/>
@@ -2656,7 +2569,7 @@
       <c r="Z65" s="1"/>
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
+      <c r="A66" s="4"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="2"/>
@@ -2684,7 +2597,7 @@
       <c r="Z66" s="1"/>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1"/>
+      <c r="A67" s="4"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="2"/>
@@ -2712,7 +2625,7 @@
       <c r="Z67" s="1"/>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1"/>
+      <c r="A68" s="4"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="2"/>
@@ -2740,7 +2653,7 @@
       <c r="Z68" s="1"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1"/>
+      <c r="A69" s="4"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="2"/>
@@ -2768,7 +2681,7 @@
       <c r="Z69" s="1"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
+      <c r="A70" s="4"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="2"/>
@@ -2796,7 +2709,7 @@
       <c r="Z70" s="1"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
+      <c r="A71" s="4"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="2"/>
@@ -2824,7 +2737,7 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
+      <c r="A72" s="4"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="2"/>
@@ -2852,7 +2765,7 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
@@ -2880,7 +2793,7 @@
       <c r="Z73" s="1"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
+      <c r="A74" s="4"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="2"/>
@@ -2908,7 +2821,7 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
@@ -28499,19 +28412,383 @@
       <c r="Y988" s="1"/>
       <c r="Z988" s="1"/>
     </row>
+    <row r="989" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A989" s="1"/>
+      <c r="B989" s="1"/>
+      <c r="C989" s="1"/>
+      <c r="D989" s="2"/>
+      <c r="E989" s="1"/>
+      <c r="F989" s="3"/>
+      <c r="G989" s="3"/>
+      <c r="H989" s="3"/>
+      <c r="I989" s="2"/>
+      <c r="J989" s="3"/>
+      <c r="K989" s="2"/>
+      <c r="L989" s="3"/>
+      <c r="M989" s="3"/>
+      <c r="N989" s="1"/>
+      <c r="O989" s="1"/>
+      <c r="P989" s="1"/>
+      <c r="Q989" s="1"/>
+      <c r="R989" s="1"/>
+      <c r="S989" s="1"/>
+      <c r="T989" s="1"/>
+      <c r="U989" s="1"/>
+      <c r="V989" s="1"/>
+      <c r="W989" s="1"/>
+      <c r="X989" s="1"/>
+      <c r="Y989" s="1"/>
+      <c r="Z989" s="1"/>
+    </row>
+    <row r="990" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A990" s="1"/>
+      <c r="B990" s="1"/>
+      <c r="C990" s="1"/>
+      <c r="D990" s="2"/>
+      <c r="E990" s="1"/>
+      <c r="F990" s="3"/>
+      <c r="G990" s="3"/>
+      <c r="H990" s="3"/>
+      <c r="I990" s="2"/>
+      <c r="J990" s="3"/>
+      <c r="K990" s="2"/>
+      <c r="L990" s="3"/>
+      <c r="M990" s="3"/>
+      <c r="N990" s="1"/>
+      <c r="O990" s="1"/>
+      <c r="P990" s="1"/>
+      <c r="Q990" s="1"/>
+      <c r="R990" s="1"/>
+      <c r="S990" s="1"/>
+      <c r="T990" s="1"/>
+      <c r="U990" s="1"/>
+      <c r="V990" s="1"/>
+      <c r="W990" s="1"/>
+      <c r="X990" s="1"/>
+      <c r="Y990" s="1"/>
+      <c r="Z990" s="1"/>
+    </row>
+    <row r="991" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A991" s="1"/>
+      <c r="B991" s="1"/>
+      <c r="C991" s="1"/>
+      <c r="D991" s="2"/>
+      <c r="E991" s="1"/>
+      <c r="F991" s="3"/>
+      <c r="G991" s="3"/>
+      <c r="H991" s="3"/>
+      <c r="I991" s="2"/>
+      <c r="J991" s="3"/>
+      <c r="K991" s="2"/>
+      <c r="L991" s="3"/>
+      <c r="M991" s="3"/>
+      <c r="N991" s="1"/>
+      <c r="O991" s="1"/>
+      <c r="P991" s="1"/>
+      <c r="Q991" s="1"/>
+      <c r="R991" s="1"/>
+      <c r="S991" s="1"/>
+      <c r="T991" s="1"/>
+      <c r="U991" s="1"/>
+      <c r="V991" s="1"/>
+      <c r="W991" s="1"/>
+      <c r="X991" s="1"/>
+      <c r="Y991" s="1"/>
+      <c r="Z991" s="1"/>
+    </row>
+    <row r="992" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A992" s="1"/>
+      <c r="B992" s="1"/>
+      <c r="C992" s="1"/>
+      <c r="D992" s="2"/>
+      <c r="E992" s="1"/>
+      <c r="F992" s="3"/>
+      <c r="G992" s="3"/>
+      <c r="H992" s="3"/>
+      <c r="I992" s="2"/>
+      <c r="J992" s="3"/>
+      <c r="K992" s="2"/>
+      <c r="L992" s="3"/>
+      <c r="M992" s="3"/>
+      <c r="N992" s="1"/>
+      <c r="O992" s="1"/>
+      <c r="P992" s="1"/>
+      <c r="Q992" s="1"/>
+      <c r="R992" s="1"/>
+      <c r="S992" s="1"/>
+      <c r="T992" s="1"/>
+      <c r="U992" s="1"/>
+      <c r="V992" s="1"/>
+      <c r="W992" s="1"/>
+      <c r="X992" s="1"/>
+      <c r="Y992" s="1"/>
+      <c r="Z992" s="1"/>
+    </row>
+    <row r="993" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A993" s="1"/>
+      <c r="B993" s="1"/>
+      <c r="C993" s="1"/>
+      <c r="D993" s="2"/>
+      <c r="E993" s="1"/>
+      <c r="F993" s="3"/>
+      <c r="G993" s="3"/>
+      <c r="H993" s="3"/>
+      <c r="I993" s="2"/>
+      <c r="J993" s="3"/>
+      <c r="K993" s="2"/>
+      <c r="L993" s="3"/>
+      <c r="M993" s="3"/>
+      <c r="N993" s="1"/>
+      <c r="O993" s="1"/>
+      <c r="P993" s="1"/>
+      <c r="Q993" s="1"/>
+      <c r="R993" s="1"/>
+      <c r="S993" s="1"/>
+      <c r="T993" s="1"/>
+      <c r="U993" s="1"/>
+      <c r="V993" s="1"/>
+      <c r="W993" s="1"/>
+      <c r="X993" s="1"/>
+      <c r="Y993" s="1"/>
+      <c r="Z993" s="1"/>
+    </row>
+    <row r="994" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A994" s="1"/>
+      <c r="B994" s="1"/>
+      <c r="C994" s="1"/>
+      <c r="D994" s="2"/>
+      <c r="E994" s="1"/>
+      <c r="F994" s="3"/>
+      <c r="G994" s="3"/>
+      <c r="H994" s="3"/>
+      <c r="I994" s="2"/>
+      <c r="J994" s="3"/>
+      <c r="K994" s="2"/>
+      <c r="L994" s="3"/>
+      <c r="M994" s="3"/>
+      <c r="N994" s="1"/>
+      <c r="O994" s="1"/>
+      <c r="P994" s="1"/>
+      <c r="Q994" s="1"/>
+      <c r="R994" s="1"/>
+      <c r="S994" s="1"/>
+      <c r="T994" s="1"/>
+      <c r="U994" s="1"/>
+      <c r="V994" s="1"/>
+      <c r="W994" s="1"/>
+      <c r="X994" s="1"/>
+      <c r="Y994" s="1"/>
+      <c r="Z994" s="1"/>
+    </row>
+    <row r="995" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A995" s="1"/>
+      <c r="B995" s="1"/>
+      <c r="C995" s="1"/>
+      <c r="D995" s="2"/>
+      <c r="E995" s="1"/>
+      <c r="F995" s="3"/>
+      <c r="G995" s="3"/>
+      <c r="H995" s="3"/>
+      <c r="I995" s="2"/>
+      <c r="J995" s="3"/>
+      <c r="K995" s="2"/>
+      <c r="L995" s="3"/>
+      <c r="M995" s="3"/>
+      <c r="N995" s="1"/>
+      <c r="O995" s="1"/>
+      <c r="P995" s="1"/>
+      <c r="Q995" s="1"/>
+      <c r="R995" s="1"/>
+      <c r="S995" s="1"/>
+      <c r="T995" s="1"/>
+      <c r="U995" s="1"/>
+      <c r="V995" s="1"/>
+      <c r="W995" s="1"/>
+      <c r="X995" s="1"/>
+      <c r="Y995" s="1"/>
+      <c r="Z995" s="1"/>
+    </row>
+    <row r="996" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A996" s="1"/>
+      <c r="B996" s="1"/>
+      <c r="C996" s="1"/>
+      <c r="D996" s="2"/>
+      <c r="E996" s="1"/>
+      <c r="F996" s="3"/>
+      <c r="G996" s="3"/>
+      <c r="H996" s="3"/>
+      <c r="I996" s="2"/>
+      <c r="J996" s="3"/>
+      <c r="K996" s="2"/>
+      <c r="L996" s="3"/>
+      <c r="M996" s="3"/>
+      <c r="N996" s="1"/>
+      <c r="O996" s="1"/>
+      <c r="P996" s="1"/>
+      <c r="Q996" s="1"/>
+      <c r="R996" s="1"/>
+      <c r="S996" s="1"/>
+      <c r="T996" s="1"/>
+      <c r="U996" s="1"/>
+      <c r="V996" s="1"/>
+      <c r="W996" s="1"/>
+      <c r="X996" s="1"/>
+      <c r="Y996" s="1"/>
+      <c r="Z996" s="1"/>
+    </row>
+    <row r="997" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A997" s="1"/>
+      <c r="B997" s="1"/>
+      <c r="C997" s="1"/>
+      <c r="D997" s="2"/>
+      <c r="E997" s="1"/>
+      <c r="F997" s="3"/>
+      <c r="G997" s="3"/>
+      <c r="H997" s="3"/>
+      <c r="I997" s="2"/>
+      <c r="J997" s="3"/>
+      <c r="K997" s="2"/>
+      <c r="L997" s="3"/>
+      <c r="M997" s="3"/>
+      <c r="N997" s="1"/>
+      <c r="O997" s="1"/>
+      <c r="P997" s="1"/>
+      <c r="Q997" s="1"/>
+      <c r="R997" s="1"/>
+      <c r="S997" s="1"/>
+      <c r="T997" s="1"/>
+      <c r="U997" s="1"/>
+      <c r="V997" s="1"/>
+      <c r="W997" s="1"/>
+      <c r="X997" s="1"/>
+      <c r="Y997" s="1"/>
+      <c r="Z997" s="1"/>
+    </row>
+    <row r="998" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A998" s="1"/>
+      <c r="B998" s="1"/>
+      <c r="C998" s="1"/>
+      <c r="D998" s="2"/>
+      <c r="E998" s="1"/>
+      <c r="F998" s="3"/>
+      <c r="G998" s="3"/>
+      <c r="H998" s="3"/>
+      <c r="I998" s="2"/>
+      <c r="J998" s="3"/>
+      <c r="K998" s="2"/>
+      <c r="L998" s="3"/>
+      <c r="M998" s="3"/>
+      <c r="N998" s="1"/>
+      <c r="O998" s="1"/>
+      <c r="P998" s="1"/>
+      <c r="Q998" s="1"/>
+      <c r="R998" s="1"/>
+      <c r="S998" s="1"/>
+      <c r="T998" s="1"/>
+      <c r="U998" s="1"/>
+      <c r="V998" s="1"/>
+      <c r="W998" s="1"/>
+      <c r="X998" s="1"/>
+      <c r="Y998" s="1"/>
+      <c r="Z998" s="1"/>
+    </row>
+    <row r="999" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A999" s="1"/>
+      <c r="B999" s="1"/>
+      <c r="C999" s="1"/>
+      <c r="D999" s="2"/>
+      <c r="E999" s="1"/>
+      <c r="F999" s="3"/>
+      <c r="G999" s="3"/>
+      <c r="H999" s="3"/>
+      <c r="I999" s="2"/>
+      <c r="J999" s="3"/>
+      <c r="K999" s="2"/>
+      <c r="L999" s="3"/>
+      <c r="M999" s="3"/>
+      <c r="N999" s="1"/>
+      <c r="O999" s="1"/>
+      <c r="P999" s="1"/>
+      <c r="Q999" s="1"/>
+      <c r="R999" s="1"/>
+      <c r="S999" s="1"/>
+      <c r="T999" s="1"/>
+      <c r="U999" s="1"/>
+      <c r="V999" s="1"/>
+      <c r="W999" s="1"/>
+      <c r="X999" s="1"/>
+      <c r="Y999" s="1"/>
+      <c r="Z999" s="1"/>
+    </row>
+    <row r="1000" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1000" s="1"/>
+      <c r="B1000" s="1"/>
+      <c r="C1000" s="1"/>
+      <c r="D1000" s="2"/>
+      <c r="E1000" s="1"/>
+      <c r="F1000" s="3"/>
+      <c r="G1000" s="3"/>
+      <c r="H1000" s="3"/>
+      <c r="I1000" s="2"/>
+      <c r="J1000" s="3"/>
+      <c r="K1000" s="2"/>
+      <c r="L1000" s="3"/>
+      <c r="M1000" s="3"/>
+      <c r="N1000" s="1"/>
+      <c r="O1000" s="1"/>
+      <c r="P1000" s="1"/>
+      <c r="Q1000" s="1"/>
+      <c r="R1000" s="1"/>
+      <c r="S1000" s="1"/>
+      <c r="T1000" s="1"/>
+      <c r="U1000" s="1"/>
+      <c r="V1000" s="1"/>
+      <c r="W1000" s="1"/>
+      <c r="X1000" s="1"/>
+      <c r="Y1000" s="1"/>
+      <c r="Z1000" s="1"/>
+    </row>
+    <row r="1001" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1001" s="1"/>
+      <c r="B1001" s="1"/>
+      <c r="C1001" s="1"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="1"/>
+      <c r="F1001" s="3"/>
+      <c r="G1001" s="3"/>
+      <c r="H1001" s="3"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="3"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="3"/>
+      <c r="M1001" s="3"/>
+      <c r="N1001" s="1"/>
+      <c r="O1001" s="1"/>
+      <c r="P1001" s="1"/>
+      <c r="Q1001" s="1"/>
+      <c r="R1001" s="1"/>
+      <c r="S1001" s="1"/>
+      <c r="T1001" s="1"/>
+      <c r="U1001" s="1"/>
+      <c r="V1001" s="1"/>
+      <c r="W1001" s="1"/>
+      <c r="X1001" s="1"/>
+      <c r="Y1001" s="1"/>
+      <c r="Z1001" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C45:C988 C1:C33" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C58:C1001 C34:C46 C1:C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F988" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E34:E1001 E1:E32" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"text,enumerated,dateTime,numeric"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F34:F1001 F1:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H988" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H34:H1001 H1:H32" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E988" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -28537,13 +28814,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>

</xml_diff>

<commit_message>
adds levels to catch metadata xslx
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17398A08-9CDD-4541-B294-B712143ABBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF3E9FD-F2A7-194A-B053-F4DDF0B51194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>Foreign Key to the CAMP Release table</t>
-  </si>
-  <si>
-    <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis.</t>
   </si>
   <si>
     <t>Origin/production type of the fish. Levels = c("Hatchery", "Natural", "Unknown")</t>
@@ -211,7 +208,10 @@
     <t>Work that was done during visit to trap. Levels = c("Continue trapping", "Start trap &amp; begin trapping", "End trapping", "Unplanned restart")</t>
   </si>
   <si>
-    <t>Common name of species</t>
+    <t>Common name of species. Levels = c("Chinook salmon", "Prickly sculpin", "Steelhead / rainbow trout", "Bluegill", "Golden shiner", "Wakasagi / Japanese smelt", "Pacific lamprey", "White crappie", "Unknown lamprey (Entosphenus or Lampetra)", "Tule perch", "Redear sunfish", "Largemouth bass", "Warmouth", "Sacramento pikeminnow", "Unknown bony fish", "Green sunfish" ,"Western mosquitofish", "Black crappie", "Threadfin shad", "Unknown sculpin (Cottus)", "Riffle sculpin" ,"Bigscale logperch" ,"Sacramento sucker", "River lamprey", "Common carp", "Smallmouth bass", "Splittail", "Redeye bass", "Hitch", "Unknown bass (Micropterus)", "Brown bullhead", "Hardhead", "Spotted bass", "Speckled dace", "Unknown sunfish (Lepomis)", "Unknown minnow", "Brook trout", "American shad", "Unknown catfish or bullhead", "Mosquitofish", "Pumpkinseed", "Black bullhead", "Channel catfish")</t>
+  </si>
+  <si>
+    <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis. Levels = c("Not recorded", "Spring", "Fall", "Late fall", "Winter")</t>
   </si>
 </sst>
 </file>
@@ -241,6 +241,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -530,7 +531,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -606,10 +607,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -682,26 +683,26 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="7"/>
@@ -722,10 +723,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -760,10 +761,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -798,10 +799,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -874,10 +875,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -950,10 +951,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -988,10 +989,10 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
@@ -1026,10 +1027,10 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
@@ -1064,10 +1065,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1102,28 +1103,28 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="5"/>
@@ -1146,26 +1147,26 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="5"/>
@@ -1188,26 +1189,26 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="5"/>
@@ -1230,10 +1231,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -28814,13 +28815,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>

</xml_diff>

<commit_message>
renames some units to EML standard
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF3E9FD-F2A7-194A-B053-F4DDF0B51194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B700AA3A-3734-9F4F-B673-5CAC49EE00FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>numeric</t>
   </si>
   <si>
-    <t>millimeters</t>
-  </si>
-  <si>
     <t>real</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis. Levels = c("Not recorded", "Spring", "Fall", "Late fall", "Winter")</t>
+  </si>
+  <si>
+    <t>millimeter</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -607,10 +607,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>13</v>
@@ -683,26 +683,26 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="7"/>
@@ -723,10 +723,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -761,10 +761,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -799,10 +799,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -875,10 +875,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -951,10 +951,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
@@ -1065,10 +1065,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
@@ -1121,10 +1121,10 @@
         <v>28</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="5"/>
@@ -1147,10 +1147,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>28</v>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="5"/>
@@ -1189,10 +1189,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>28</v>
@@ -1208,7 +1208,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="5"/>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -28815,13 +28815,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>

</xml_diff>

<commit_message>
fills in units and adds custom units to make_metadata_xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B700AA3A-3734-9F4F-B673-5CAC49EE00FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A5D23-3E60-5F4F-BEEB-4914BB0245E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="63">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>millimeter</t>
+  </si>
+  <si>
+    <t>number of fish</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1164,7 +1167,9 @@
       <c r="F16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="H16" s="3" t="s">
         <v>35</v>
       </c>
@@ -1206,7 +1211,9 @@
       <c r="F17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="H17" s="3" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
adds min/max for numeric attributes
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A5D23-3E60-5F4F-BEEB-4914BB0245E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A593F3-CEFE-A549-B3C2-144C289D6822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,9 +163,6 @@
     <t>Foreign key to the CAMP ProjectDescription table. All data associated with this package will have a ProjectDescriptionID = 2</t>
   </si>
   <si>
-    <t>YYYY-MM-DD</t>
-  </si>
-  <si>
     <t>ProjectDescriptionID</t>
   </si>
   <si>
@@ -216,11 +213,17 @@
   <si>
     <t>number of fish</t>
   </si>
+  <si>
+    <t>YYYY-MM-DD hh:mm:ss</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -286,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -313,6 +316,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -534,7 +544,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -550,7 +560,7 @@
     <col min="9" max="9" width="14.1640625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" customWidth="1"/>
+    <col min="12" max="13" width="16" bestFit="1" customWidth="1"/>
     <col min="14" max="26" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -610,7 +620,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>44</v>
@@ -705,11 +715,15 @@
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
-      <c r="K4" s="6"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="3"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="13">
+        <v>35786.444444444445</v>
+      </c>
+      <c r="M4" s="13">
+        <v>38743.416666666664</v>
+      </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -726,10 +740,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -764,10 +778,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -802,10 +816,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -878,10 +892,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -954,10 +968,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -992,7 +1006,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>24</v>
@@ -1030,7 +1044,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>25</v>
@@ -1068,7 +1082,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>37</v>
@@ -1124,7 +1138,7 @@
         <v>28</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>30</v>
@@ -1132,8 +1146,12 @@
       <c r="I15" s="2"/>
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="3"/>
+      <c r="L15" s="14">
+        <v>2</v>
+      </c>
+      <c r="M15" s="14">
+        <v>910</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1168,7 +1186,7 @@
         <v>28</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>35</v>
@@ -1176,8 +1194,12 @@
       <c r="I16" s="2"/>
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="3"/>
+      <c r="L16" s="14">
+        <v>7</v>
+      </c>
+      <c r="M16" s="3">
+        <v>700</v>
+      </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1212,7 +1234,7 @@
         <v>28</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>30</v>
@@ -1220,8 +1242,12 @@
       <c r="I17" s="2"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="3"/>
+      <c r="L17" s="14">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <v>59347</v>
+      </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1238,7 +1264,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
updates metadata, xml validates
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43760072-2178-C245-9BD9-D907A6E884EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4627A319-FED9-D24E-AE29-8098874F304C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8300" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9440" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -215,9 +215,6 @@
   </si>
   <si>
     <t>Feather River RST program</t>
-  </si>
-  <si>
-    <t>projectDescriptionID</t>
   </si>
   <si>
     <t>enumerated</t>
@@ -548,9 +545,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -638,7 +635,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -28840,8 +28837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28894,7 +28891,7 @@
         <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
updates attribute to match data, validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4627A319-FED9-D24E-AE29-8098874F304C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722655C3-480D-A240-81DB-3BD2E4CD30C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9440" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9440" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -181,9 +181,6 @@
     <t>fishOrigin</t>
   </si>
   <si>
-    <t>lifestage</t>
-  </si>
-  <si>
     <t>mort</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>enumerated</t>
+  </si>
+  <si>
+    <t>lifeStage</t>
   </si>
 </sst>
 </file>
@@ -545,9 +545,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -635,7 +635,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -718,7 +718,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="13">
@@ -746,7 +746,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -784,7 +784,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -822,7 +822,7 @@
         <v>47</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -898,7 +898,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -974,7 +974,7 @@
         <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>36</v>
@@ -1141,7 +1141,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>29</v>
@@ -1189,7 +1189,7 @@
         <v>27</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>34</v>
@@ -1237,7 +1237,7 @@
         <v>27</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>29</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>35</v>
@@ -28837,7 +28837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -28888,7 +28888,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
updates trap & catch data w/ new files 12-19. xml validates.
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722655C3-480D-A240-81DB-3BD2E4CD30C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E489970-A98D-7D42-B454-73536E77D8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9440" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31700" yWindow="-21020" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -725,7 +725,7 @@
         <v>35786.444444444445</v>
       </c>
       <c r="M4" s="13">
-        <v>38743.416666666664</v>
+        <v>44902.361516203702</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -1150,10 +1150,10 @@
       <c r="J15" s="5"/>
       <c r="K15" s="6"/>
       <c r="L15" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M15" s="14">
-        <v>910</v>
+        <v>940</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1198,10 +1198,10 @@
       <c r="J16" s="5"/>
       <c r="K16" s="6"/>
       <c r="L16" s="14">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M16" s="3">
-        <v>700</v>
+        <v>750</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1249,7 +1249,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="3">
-        <v>59347</v>
+        <v>123556</v>
       </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>

</xml_diff>

<commit_message>
updates tables with new tables 3-29-2023
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E489970-A98D-7D42-B454-73536E77D8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B686FE69-708B-1745-BE0F-B38A03DC00F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31700" yWindow="-21020" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>Common name of species. Levels = c("Chinook salmon", "Prickly sculpin", "Steelhead / rainbow trout", "Bluegill", "Golden shiner", "Wakasagi / Japanese smelt", "Pacific lamprey", "White crappie", "Unknown lamprey (Entosphenus or Lampetra)", "Tule perch", "Redear sunfish", "Largemouth bass", "Warmouth", "Sacramento pikeminnow", "Unknown bony fish", "Green sunfish" ,"Western mosquitofish", "Black crappie", "Threadfin shad", "Unknown sculpin (Cottus)", "Riffle sculpin" ,"Bigscale logperch" ,"Sacramento sucker", "River lamprey", "Common carp", "Smallmouth bass", "Splittail", "Redeye bass", "Hitch", "Unknown bass (Micropterus)", "Brown bullhead", "Hardhead", "Spotted bass", "Speckled dace", "Unknown sunfish (Lepomis)", "Unknown minnow", "Brook trout", "American shad", "Unknown catfish or bullhead", "Mosquitofish", "Pumpkinseed", "Black bullhead", "Channel catfish")</t>
   </si>
   <si>
-    <t>Run designation as determined in the field or as assigned at a later date. This is the field used in analysis. Levels = c("Not recorded", "Spring", "Fall", "Late fall", "Winter")</t>
-  </si>
-  <si>
     <t>millimeter</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>lifeStage</t>
+  </si>
+  <si>
+    <t>Run designation as determined in the field or as assigned at a later date.  Levels = c("Not recorded", "Spring", "Fall", "Late fall", "Winter")</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -635,7 +635,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -718,7 +718,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="13">
@@ -974,7 +974,7 @@
         <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -1141,7 +1141,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>29</v>
@@ -1189,7 +1189,7 @@
         <v>27</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>34</v>
@@ -1237,7 +1237,7 @@
         <v>27</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>29</v>
@@ -28888,7 +28888,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
updates metadata tables for new data tables
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B686FE69-708B-1745-BE0F-B38A03DC00F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4795C2-5EBC-C64C-B479-4C2885EE7E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="62">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -136,9 +136,6 @@
     <t>Whether the count (n) is an actual count or estimate. Levels = c("Yes", "No")</t>
   </si>
   <si>
-    <t>Whether fish died due to being captured or handled.  Levels = c("Yes", "No")</t>
-  </si>
-  <si>
     <t>visitTime</t>
   </si>
   <si>
@@ -179,9 +176,6 @@
   </si>
   <si>
     <t>fishOrigin</t>
-  </si>
-  <si>
-    <t>mort</t>
   </si>
   <si>
     <t>ActualCount</t>
@@ -543,11 +537,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -623,10 +617,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>17</v>
@@ -635,7 +629,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -699,33 +693,33 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="13">
         <v>35786.444444444445</v>
       </c>
       <c r="M4" s="13">
-        <v>44902.361516203702</v>
+        <v>44990.427511574075</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -743,10 +737,10 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -781,10 +775,10 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -819,10 +813,10 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -895,10 +889,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -971,10 +965,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -1009,7 +1003,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
@@ -1047,7 +1041,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -1085,28 +1079,38 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="5"/>
       <c r="K14" s="6"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="14">
+        <v>3835</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1123,10 +1127,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>27</v>
@@ -1141,10 +1145,10 @@
         <v>27</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="5"/>
@@ -1152,8 +1156,8 @@
       <c r="L15" s="14">
         <v>0</v>
       </c>
-      <c r="M15" s="14">
-        <v>940</v>
+      <c r="M15" s="3">
+        <v>750</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1171,10 +1175,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>27</v>
@@ -1189,10 +1193,10 @@
         <v>27</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="5"/>
@@ -1201,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="3">
-        <v>750</v>
+        <v>123556</v>
       </c>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1219,38 +1223,28 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="2"/>
       <c r="J17" s="5"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="14">
-        <v>0</v>
-      </c>
-      <c r="M17" s="3">
-        <v>123556</v>
-      </c>
+      <c r="L17" s="7"/>
+      <c r="M17" s="3"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1266,28 +1260,18 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="2"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="7"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1387,9 +1371,8 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
@@ -1415,8 +1398,9 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
+      <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
@@ -1584,34 +1568,34 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
-      <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
+      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="1"/>
@@ -1643,39 +1627,29 @@
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="4"/>
-      <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-      <c r="X31" s="4"/>
-      <c r="Y31" s="4"/>
-      <c r="Z31" s="4"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="3"/>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1694,6 +1668,16 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="3"/>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1824,7 +1808,6 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1852,6 +1835,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -1879,7 +1863,6 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
@@ -1907,6 +1890,7 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="4"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
@@ -2858,7 +2842,7 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4"/>
+      <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="2"/>
@@ -28785,46 +28769,18 @@
       <c r="Y1000" s="1"/>
       <c r="Z1000" s="1"/>
     </row>
-    <row r="1001" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1001" s="1"/>
-      <c r="B1001" s="1"/>
-      <c r="C1001" s="1"/>
-      <c r="D1001" s="2"/>
-      <c r="E1001" s="1"/>
-      <c r="F1001" s="3"/>
-      <c r="G1001" s="3"/>
-      <c r="H1001" s="3"/>
-      <c r="I1001" s="2"/>
-      <c r="J1001" s="3"/>
-      <c r="K1001" s="2"/>
-      <c r="L1001" s="3"/>
-      <c r="M1001" s="3"/>
-      <c r="N1001" s="1"/>
-      <c r="O1001" s="1"/>
-      <c r="P1001" s="1"/>
-      <c r="Q1001" s="1"/>
-      <c r="R1001" s="1"/>
-      <c r="S1001" s="1"/>
-      <c r="T1001" s="1"/>
-      <c r="U1001" s="1"/>
-      <c r="V1001" s="1"/>
-      <c r="W1001" s="1"/>
-      <c r="X1001" s="1"/>
-      <c r="Y1001" s="1"/>
-      <c r="Z1001" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C58:C1001 C34:C46 C1:C32" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C57:C1000 C33:C45 C1:C31" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E34:E1001 E1:E32" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E33:E1000 E1:E31" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F34:F1001 F1:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F33:F1000 F1:F31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H34:H1001 H1:H32" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H33:H1000 H1:H31" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28851,13 +28807,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
@@ -28888,10 +28844,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>

</xml_diff>

<commit_message>
updates url to new SRJPE repo and fixes metadata atrribute name to match data
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_catch_metadata.xlsx
+++ b/data-raw/metadata/feather_catch_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-feather-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-feather-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4795C2-5EBC-C64C-B479-4C2885EE7E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8296F5DC-6977-2347-9858-9FB4AC617D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="180" yWindow="520" windowWidth="28800" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -178,9 +178,6 @@
     <t>fishOrigin</t>
   </si>
   <si>
-    <t>ActualCount</t>
-  </si>
-  <si>
     <t>Name of the sampling site. Levels = c("Eye Riffle", "Live Oak", "Herringer Riffle")</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
   </si>
   <si>
     <t>Run designation as determined in the field or as assigned at a later date.  Levels = c("Not recorded", "Spring", "Fall", "Late fall", "Winter")</t>
+  </si>
+  <si>
+    <t>actualCount</t>
   </si>
 </sst>
 </file>
@@ -539,9 +539,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -629,7 +629,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -712,7 +712,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K4" s="12"/>
       <c r="L4" s="13">
@@ -740,7 +740,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -778,7 +778,7 @@
         <v>45</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -816,7 +816,7 @@
         <v>46</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -892,7 +892,7 @@
         <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -968,7 +968,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
@@ -1097,7 +1097,7 @@
         <v>27</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>29</v>
@@ -1145,7 +1145,7 @@
         <v>27</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>34</v>
@@ -1193,7 +1193,7 @@
         <v>27</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>29</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>35</v>
@@ -28844,7 +28844,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>43</v>

</xml_diff>